<commit_message>
feat: introduce duckDB notebook
</commit_message>
<xml_diff>
--- a/ingested/diagnostics.xlsx
+++ b/ingested/diagnostics.xlsx
@@ -39,205 +39,205 @@
     <t>elaboration</t>
   </si>
   <si>
-    <t>2978026b-0fda-4262-b561-bc044506f484</t>
-  </si>
-  <si>
-    <t>1fa45300-5b92-4e83-bfec-6a706d0404c1</t>
+    <t>c8daea83-fb7b-4236-b2d4-75329c45d9e1</t>
+  </si>
+  <si>
+    <t>6aebd5b8-c1b6-4afb-b160-6328bd174c01</t>
   </si>
   <si>
     <t>Missing Column</t>
   </si>
   <si>
-    <t>Required column PAT_MRN_ID is missing in synthetic_fail2.</t>
-  </si>
-  <si>
-    <t>Ensure synthetic_fail2 contains the column "PAT_MRN_ID"</t>
-  </si>
-  <si>
-    <t>1c924840-0d00-471b-9e44-89cf92728327</t>
-  </si>
-  <si>
-    <t>Required column FACILITY is missing in synthetic_fail2.</t>
-  </si>
-  <si>
-    <t>Ensure synthetic_fail2 contains the column "FACILITY"</t>
-  </si>
-  <si>
-    <t>b1c4f6b5-8521-439f-9520-e3810c06c26c</t>
-  </si>
-  <si>
-    <t>Required column FIRST_NAME is missing in synthetic_fail2.</t>
-  </si>
-  <si>
-    <t>Ensure synthetic_fail2 contains the column "FIRST_NAME"</t>
-  </si>
-  <si>
-    <t>40a8fa5a-8461-4bb2-b68d-66bdee3698ae</t>
-  </si>
-  <si>
-    <t>Required column LAST_NAME is missing in synthetic_fail2.</t>
-  </si>
-  <si>
-    <t>Ensure synthetic_fail2 contains the column "LAST_NAME"</t>
-  </si>
-  <si>
-    <t>409b9f80-777e-4ab5-b76b-db2714ed60af</t>
-  </si>
-  <si>
-    <t>Required column PAT_BIRTH_DATE is missing in synthetic_fail2.</t>
-  </si>
-  <si>
-    <t>Ensure synthetic_fail2 contains the column "PAT_BIRTH_DATE"</t>
-  </si>
-  <si>
-    <t>960f9eff-8446-43c0-bb51-0673b3801014</t>
-  </si>
-  <si>
-    <t>Required column MEDICAID_CIN is missing in synthetic_fail2.</t>
-  </si>
-  <si>
-    <t>Ensure synthetic_fail2 contains the column "MEDICAID_CIN"</t>
-  </si>
-  <si>
-    <t>c1e4caf8-1783-47b4-9123-ef56c661062a</t>
-  </si>
-  <si>
-    <t>Required column ENCOUNTER_ID is missing in synthetic_fail2.</t>
-  </si>
-  <si>
-    <t>Ensure synthetic_fail2 contains the column "ENCOUNTER_ID"</t>
-  </si>
-  <si>
-    <t>df6ce432-be47-42e7-a2f6-3f971a5bef14</t>
-  </si>
-  <si>
-    <t>Required column SURVEY is missing in synthetic_fail2.</t>
-  </si>
-  <si>
-    <t>Ensure synthetic_fail2 contains the column "SURVEY"</t>
-  </si>
-  <si>
-    <t>34da6535-0f68-41f5-a08b-df356a46c1b1</t>
-  </si>
-  <si>
-    <t>Required column SURVEY_ID is missing in synthetic_fail2.</t>
-  </si>
-  <si>
-    <t>Ensure synthetic_fail2 contains the column "SURVEY_ID"</t>
-  </si>
-  <si>
-    <t>57479769-963c-4df2-9da5-d85574f32c38</t>
-  </si>
-  <si>
-    <t>Required column RECORDED_TIME is missing in synthetic_fail2.</t>
-  </si>
-  <si>
-    <t>Ensure synthetic_fail2 contains the column "RECORDED_TIME"</t>
-  </si>
-  <si>
-    <t>7ae54f82-e406-4102-a6d9-2de6889bf39e</t>
-  </si>
-  <si>
-    <t>Required column QUESTION is missing in synthetic_fail2.</t>
-  </si>
-  <si>
-    <t>Ensure synthetic_fail2 contains the column "QUESTION"</t>
-  </si>
-  <si>
-    <t>dab5521d-15ea-46d7-a77b-7d5c528d6230</t>
-  </si>
-  <si>
-    <t>Required column MEAS_VALUE is missing in synthetic_fail2.</t>
-  </si>
-  <si>
-    <t>Ensure synthetic_fail2 contains the column "MEAS_VALUE"</t>
-  </si>
-  <si>
-    <t>9c5cddea-2715-425a-8e20-8267f27e12ad</t>
-  </si>
-  <si>
-    <t>Required column QUESTION_CODE is missing in synthetic_fail2.</t>
-  </si>
-  <si>
-    <t>Ensure synthetic_fail2 contains the column "QUESTION_CODE"</t>
-  </si>
-  <si>
-    <t>9b03368d-b35d-408b-b32a-3205ece9eb22</t>
-  </si>
-  <si>
-    <t>Required column QUESTION_CODE_SYSTEM_NAME is missing in synthetic_fail2.</t>
-  </si>
-  <si>
-    <t>Ensure synthetic_fail2 contains the column "QUESTION_CODE_SYSTEM_NAME"</t>
-  </si>
-  <si>
-    <t>b6f19390-580f-46ee-9e93-27d542ecb256</t>
-  </si>
-  <si>
-    <t>Required column ANSWER_CODE is missing in synthetic_fail2.</t>
-  </si>
-  <si>
-    <t>Ensure synthetic_fail2 contains the column "ANSWER_CODE"</t>
-  </si>
-  <si>
-    <t>c654178b-16f3-405d-85cd-bd7796fd1e65</t>
-  </si>
-  <si>
-    <t>Required column ANSWER_CODE_SYSTEM_NAME is missing in synthetic_fail2.</t>
-  </si>
-  <si>
-    <t>Ensure synthetic_fail2 contains the column "ANSWER_CODE_SYSTEM_NAME"</t>
-  </si>
-  <si>
-    <t>8eab0b12-c0cf-45ec-b3c9-f1451d9de61a</t>
-  </si>
-  <si>
-    <t>Required column SDOH_DOMAIN is missing in synthetic_fail2.</t>
-  </si>
-  <si>
-    <t>Ensure synthetic_fail2 contains the column "SDOH_DOMAIN"</t>
-  </si>
-  <si>
-    <t>65df93a7-1697-446b-954f-fcf467c11baf</t>
-  </si>
-  <si>
-    <t>Required column NEED_INDICATED is missing in synthetic_fail2.</t>
-  </si>
-  <si>
-    <t>Ensure synthetic_fail2 contains the column "NEED_INDICATED"</t>
-  </si>
-  <si>
-    <t>08c6a65a-b7db-4c16-8174-47932c538eb1</t>
-  </si>
-  <si>
-    <t>Required column VISIT_PART_2_FLAG is missing in synthetic_fail2.</t>
-  </si>
-  <si>
-    <t>Ensure synthetic_fail2 contains the column "VISIT_PART_2_FLAG"</t>
-  </si>
-  <si>
-    <t>04dbc52a-e5e3-4ad6-a818-baf8ea3606bc</t>
-  </si>
-  <si>
-    <t>Required column VISIT_OMH_FLAG is missing in synthetic_fail2.</t>
-  </si>
-  <si>
-    <t>Ensure synthetic_fail2 contains the column "VISIT_OMH_FLAG"</t>
-  </si>
-  <si>
-    <t>5ee48c31-5e1d-4c69-8d01-78081cedc548</t>
-  </si>
-  <si>
-    <t>Required column VISIT_OPWDD_FLAG is missing in synthetic_fail2.</t>
-  </si>
-  <si>
-    <t>Ensure synthetic_fail2 contains the column "VISIT_OPWDD_FLAG"</t>
-  </si>
-  <si>
-    <t>a55a1969-db41-46f3-808b-d25ca2bc8d10</t>
-  </si>
-  <si>
-    <t>6c221a37-e6ea-4729-aa9f-0ce1569886c6</t>
+    <t>Required column PAT_MRN_ID is missing in synthetic_fail.</t>
+  </si>
+  <si>
+    <t>Ensure synthetic_fail contains the column "PAT_MRN_ID"</t>
+  </si>
+  <si>
+    <t>5231d332-934f-41a1-bf3a-bf4e729f91b7</t>
+  </si>
+  <si>
+    <t>Required column FACILITY is missing in synthetic_fail.</t>
+  </si>
+  <si>
+    <t>Ensure synthetic_fail contains the column "FACILITY"</t>
+  </si>
+  <si>
+    <t>1f312a3c-27fb-432b-a263-e438e4185b71</t>
+  </si>
+  <si>
+    <t>Required column FIRST_NAME is missing in synthetic_fail.</t>
+  </si>
+  <si>
+    <t>Ensure synthetic_fail contains the column "FIRST_NAME"</t>
+  </si>
+  <si>
+    <t>455b2050-381b-4964-8752-4143755e6996</t>
+  </si>
+  <si>
+    <t>Required column LAST_NAME is missing in synthetic_fail.</t>
+  </si>
+  <si>
+    <t>Ensure synthetic_fail contains the column "LAST_NAME"</t>
+  </si>
+  <si>
+    <t>f56834d4-40cf-478c-a4ba-bec92cc59265</t>
+  </si>
+  <si>
+    <t>Required column PAT_BIRTH_DATE is missing in synthetic_fail.</t>
+  </si>
+  <si>
+    <t>Ensure synthetic_fail contains the column "PAT_BIRTH_DATE"</t>
+  </si>
+  <si>
+    <t>15868a63-eb31-47a5-9f55-0e71d000c03c</t>
+  </si>
+  <si>
+    <t>Required column MEDICAID_CIN is missing in synthetic_fail.</t>
+  </si>
+  <si>
+    <t>Ensure synthetic_fail contains the column "MEDICAID_CIN"</t>
+  </si>
+  <si>
+    <t>b9d0988e-afd8-4443-9df7-0dd02884df1a</t>
+  </si>
+  <si>
+    <t>Required column ENCOUNTER_ID is missing in synthetic_fail.</t>
+  </si>
+  <si>
+    <t>Ensure synthetic_fail contains the column "ENCOUNTER_ID"</t>
+  </si>
+  <si>
+    <t>847381c1-561e-4a4f-afa7-b2851202b04b</t>
+  </si>
+  <si>
+    <t>Required column SURVEY is missing in synthetic_fail.</t>
+  </si>
+  <si>
+    <t>Ensure synthetic_fail contains the column "SURVEY"</t>
+  </si>
+  <si>
+    <t>1b9a9bef-7f28-43e1-8956-454bc775cf77</t>
+  </si>
+  <si>
+    <t>Required column SURVEY_ID is missing in synthetic_fail.</t>
+  </si>
+  <si>
+    <t>Ensure synthetic_fail contains the column "SURVEY_ID"</t>
+  </si>
+  <si>
+    <t>23df3b39-347d-4091-a2ef-77c6ee3256f8</t>
+  </si>
+  <si>
+    <t>Required column RECORDED_TIME is missing in synthetic_fail.</t>
+  </si>
+  <si>
+    <t>Ensure synthetic_fail contains the column "RECORDED_TIME"</t>
+  </si>
+  <si>
+    <t>bb2504c7-0bb5-4664-bc49-1a233a0aa321</t>
+  </si>
+  <si>
+    <t>Required column QUESTION is missing in synthetic_fail.</t>
+  </si>
+  <si>
+    <t>Ensure synthetic_fail contains the column "QUESTION"</t>
+  </si>
+  <si>
+    <t>53171127-f04a-420a-9c19-9dc87d3dad33</t>
+  </si>
+  <si>
+    <t>Required column MEAS_VALUE is missing in synthetic_fail.</t>
+  </si>
+  <si>
+    <t>Ensure synthetic_fail contains the column "MEAS_VALUE"</t>
+  </si>
+  <si>
+    <t>42fee73a-c3f5-450e-af0b-84f3a945e3c9</t>
+  </si>
+  <si>
+    <t>Required column QUESTION_CODE is missing in synthetic_fail.</t>
+  </si>
+  <si>
+    <t>Ensure synthetic_fail contains the column "QUESTION_CODE"</t>
+  </si>
+  <si>
+    <t>db2f4386-3e01-4852-94da-bfcabe69edf9</t>
+  </si>
+  <si>
+    <t>Required column QUESTION_CODE_SYSTEM_NAME is missing in synthetic_fail.</t>
+  </si>
+  <si>
+    <t>Ensure synthetic_fail contains the column "QUESTION_CODE_SYSTEM_NAME"</t>
+  </si>
+  <si>
+    <t>623332c5-6c98-48e6-a314-fff385e13377</t>
+  </si>
+  <si>
+    <t>Required column ANSWER_CODE is missing in synthetic_fail.</t>
+  </si>
+  <si>
+    <t>Ensure synthetic_fail contains the column "ANSWER_CODE"</t>
+  </si>
+  <si>
+    <t>3cc08034-c98a-4bf4-a43d-715c19513897</t>
+  </si>
+  <si>
+    <t>Required column ANSWER_CODE_SYSTEM_NAME is missing in synthetic_fail.</t>
+  </si>
+  <si>
+    <t>Ensure synthetic_fail contains the column "ANSWER_CODE_SYSTEM_NAME"</t>
+  </si>
+  <si>
+    <t>0eb487b4-92a3-4aca-b2db-dd9925dac12b</t>
+  </si>
+  <si>
+    <t>Required column SDOH_DOMAIN is missing in synthetic_fail.</t>
+  </si>
+  <si>
+    <t>Ensure synthetic_fail contains the column "SDOH_DOMAIN"</t>
+  </si>
+  <si>
+    <t>37ad9a18-3b78-4efe-93ca-583262a46cfd</t>
+  </si>
+  <si>
+    <t>Required column NEED_INDICATED is missing in synthetic_fail.</t>
+  </si>
+  <si>
+    <t>Ensure synthetic_fail contains the column "NEED_INDICATED"</t>
+  </si>
+  <si>
+    <t>68eeaf59-3b60-4bf4-89e1-7ea93c100d82</t>
+  </si>
+  <si>
+    <t>Required column VISIT_PART_2_FLAG is missing in synthetic_fail.</t>
+  </si>
+  <si>
+    <t>Ensure synthetic_fail contains the column "VISIT_PART_2_FLAG"</t>
+  </si>
+  <si>
+    <t>37e84512-2d22-44b4-ab8c-140f347f606e</t>
+  </si>
+  <si>
+    <t>Required column VISIT_OMH_FLAG is missing in synthetic_fail.</t>
+  </si>
+  <si>
+    <t>Ensure synthetic_fail contains the column "VISIT_OMH_FLAG"</t>
+  </si>
+  <si>
+    <t>c7111633-b226-4b9c-b4e6-d7cfc60c527f</t>
+  </si>
+  <si>
+    <t>Required column VISIT_OPWDD_FLAG is missing in synthetic_fail.</t>
+  </si>
+  <si>
+    <t>Ensure synthetic_fail contains the column "VISIT_OPWDD_FLAG"</t>
+  </si>
+  <si>
+    <t>a37edbfa-bbf2-4a73-8118-653367661f25</t>
+  </si>
+  <si>
+    <t>9b5ab88a-e757-4520-b89f-b64c440235e1</t>
   </si>
   <si>
     <t>Data Type Mismatch</t>
@@ -255,82 +255,82 @@
     <t>Convert non-integer values to INTEGER</t>
   </si>
   <si>
-    <t>676dd16e-de56-47df-ad3f-9df74c34d5da</t>
-  </si>
-  <si>
-    <t>e21ec4e0-816a-4d1d-8543-7a1b92afdca2</t>
-  </si>
-  <si>
-    <t>893dde99-42e1-4917-bbe7-d8b65139ebe0</t>
-  </si>
-  <si>
-    <t>319d4ab9-224d-4b9c-8849-f81646e8d23c</t>
-  </si>
-  <si>
-    <t>4b284ee0-e792-49bd-a10b-75c613b3056a</t>
-  </si>
-  <si>
-    <t>0a59f1c4-d873-44bb-b73b-3ed9a35b8476</t>
-  </si>
-  <si>
-    <t>3e7c04a0-7194-4c71-a3d7-a796130cfcd5</t>
-  </si>
-  <si>
-    <t>1c739627-7b05-40a4-b63f-6d47af293290</t>
-  </si>
-  <si>
-    <t>ea90154b-e033-42a3-920b-33589943dc00</t>
-  </si>
-  <si>
-    <t>a89412d3-42b5-4a4e-91aa-ddb6e08b8383</t>
-  </si>
-  <si>
-    <t>db56979b-3b5d-4d59-a297-c49e3d327eb4</t>
-  </si>
-  <si>
-    <t>6a0f05e7-a196-453d-8f86-4cdbc3c4f8fb</t>
-  </si>
-  <si>
-    <t>af868152-6b81-4e37-adcd-0a039dc85ac7</t>
-  </si>
-  <si>
-    <t>735f8bcd-ef7c-452f-964e-ec19df8a1ab1</t>
-  </si>
-  <si>
-    <t>4122925d-e8c2-41f0-b856-a4862006d3e8</t>
-  </si>
-  <si>
-    <t>28146082-40e4-4b45-9284-84b716092a94</t>
-  </si>
-  <si>
-    <t>59fb172d-71d6-4625-8bb1-d7b1f091355a</t>
-  </si>
-  <si>
-    <t>3cd0a73f-c5e9-432c-b214-c00f9eba2231</t>
-  </si>
-  <si>
-    <t>8f1f2df6-d058-43c1-ad3e-5825973dbe94</t>
-  </si>
-  <si>
-    <t>d61192de-0155-4c76-bb58-f9a88b1628d6</t>
-  </si>
-  <si>
-    <t>1f464b4f-edc1-4151-84a6-91dd38fb19b4</t>
-  </si>
-  <si>
-    <t>1ae2df18-87b9-4fe0-ad47-e522567de276</t>
-  </si>
-  <si>
-    <t>e6bd381f-e200-4c97-b573-c34dc1c3d6a1</t>
-  </si>
-  <si>
-    <t>f0a3fe29-360f-4146-b610-f026fb93af76</t>
-  </si>
-  <si>
-    <t>0b554e4e-6bd6-4a84-b35a-846bb1639e83</t>
-  </si>
-  <si>
-    <t>64f714e9-ec9f-4de6-b6d5-542988d63d14</t>
+    <t>ae575048-b0e8-4291-8624-46ba902f789a</t>
+  </si>
+  <si>
+    <t>77a53eda-afa2-4397-91da-383519fbc6d1</t>
+  </si>
+  <si>
+    <t>d1ac8450-64a2-4d30-9f3f-7fd2aacb844c</t>
+  </si>
+  <si>
+    <t>ce6f461e-3541-477b-a164-076e9a297ef4</t>
+  </si>
+  <si>
+    <t>c8f72ba0-1375-4520-8b44-4150b97064c4</t>
+  </si>
+  <si>
+    <t>2b30fb94-3126-47b0-9fe1-d44c10cdf9d1</t>
+  </si>
+  <si>
+    <t>6bf5c7b1-f1a3-42a2-98b6-cb77e73a1937</t>
+  </si>
+  <si>
+    <t>e9b098a6-0919-4a58-a56c-5dc3499ec3d8</t>
+  </si>
+  <si>
+    <t>3c088bdc-4d7f-44e2-8215-bcffd4f276c3</t>
+  </si>
+  <si>
+    <t>26f8f051-6a39-4443-ba4f-a0bd190d4716</t>
+  </si>
+  <si>
+    <t>360da663-a72b-4a41-ba76-8a04f4f91087</t>
+  </si>
+  <si>
+    <t>52384fea-97e9-4972-b19f-c0be0bbbcddf</t>
+  </si>
+  <si>
+    <t>cac8fdb1-af13-4e47-b49c-341538522788</t>
+  </si>
+  <si>
+    <t>25e9ef0e-1757-4ceb-b731-bfe8f6c45f82</t>
+  </si>
+  <si>
+    <t>8e3cba8c-8a00-4b58-8cab-9e2a779ea4c1</t>
+  </si>
+  <si>
+    <t>58044080-ee49-496f-9250-2f0b7a286b68</t>
+  </si>
+  <si>
+    <t>240e19b6-c5e8-46d5-aac8-85eb9e0d9882</t>
+  </si>
+  <si>
+    <t>aac362d8-023c-4b19-9133-753c504b5ae7</t>
+  </si>
+  <si>
+    <t>c426f50f-7047-4f57-b304-8aaec3d8f36f</t>
+  </si>
+  <si>
+    <t>973489ba-cfad-4852-b657-4f85963ec05b</t>
+  </si>
+  <si>
+    <t>9427ced5-0090-4d82-961f-f5608593becd</t>
+  </si>
+  <si>
+    <t>19bd9ff7-1b18-4c9a-b80d-758e90a7a4be</t>
+  </si>
+  <si>
+    <t>0285beed-bcbe-442d-8022-417c4c938b58</t>
+  </si>
+  <si>
+    <t>53ea0150-5235-4659-897d-9937f29bd2bb</t>
+  </si>
+  <si>
+    <t>7ddef889-dd34-4913-9690-5baf7eeef4ee</t>
+  </si>
+  <si>
+    <t>2d502869-a85e-4f26-928b-12ec67e5d498</t>
   </si>
 </sst>
 </file>

</xml_diff>